<commit_message>
Made presentation and updated scripts
</commit_message>
<xml_diff>
--- a/References /LitReview.xlsx
+++ b/References /LitReview.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/falsespring/References /"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27430"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20260" yWindow="1060" windowWidth="26320" windowHeight="21120" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -17,20 +12,23 @@
     <sheet name="papers" sheetId="3" r:id="rId3"/>
     <sheet name="scratch" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">papers!$A$1:$W$1</definedName>
+  </definedNames>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="140">
   <si>
     <t>Metadata by Cat:</t>
   </si>
@@ -444,13 +442,19 @@
   </si>
   <si>
     <t>vitasse14</t>
+  </si>
+  <si>
+    <t>basler12</t>
+  </si>
+  <si>
+    <t>fu12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -493,6 +497,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -511,8 +531,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -527,7 +551,11 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -583,7 +611,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -618,7 +646,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -795,7 +823,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -809,27 +837,27 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -841,7 +869,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
@@ -850,7 +878,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
@@ -862,7 +890,7 @@
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="19">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -874,7 +902,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="19">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -888,7 +916,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="19">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -902,7 +930,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="19">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -916,7 +944,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="17">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -926,7 +954,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="19">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -938,7 +966,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="19">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -952,7 +980,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="19">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -966,7 +994,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="19">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -980,7 +1008,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="19">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -994,7 +1022,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="19">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
@@ -1008,7 +1036,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="19">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1022,7 +1050,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="17">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1032,7 +1060,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="19">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1044,7 +1072,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="19">
       <c r="A23" s="4" t="s">
         <v>74</v>
       </c>
@@ -1058,7 +1086,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="19">
       <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
@@ -1072,7 +1100,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="19">
       <c r="A25" s="4" t="s">
         <v>28</v>
       </c>
@@ -1084,7 +1112,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="19">
       <c r="A26" s="4" t="s">
         <v>29</v>
       </c>
@@ -1096,7 +1124,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="19">
       <c r="A27" s="4" t="s">
         <v>30</v>
       </c>
@@ -1108,7 +1136,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="19">
       <c r="A28" s="4" t="s">
         <v>31</v>
       </c>
@@ -1120,7 +1148,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="19">
       <c r="A29" s="4" t="s">
         <v>32</v>
       </c>
@@ -1132,7 +1160,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="19">
       <c r="A30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1140,7 +1168,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="19">
       <c r="A31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1148,7 +1176,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="19">
       <c r="A32" s="4" t="s">
         <v>64</v>
       </c>
@@ -1156,7 +1184,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="19">
       <c r="A33" s="4" t="s">
         <v>66</v>
       </c>
@@ -1164,7 +1192,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="19">
       <c r="A34" s="4" t="s">
         <v>69</v>
       </c>
@@ -1172,7 +1200,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="19">
       <c r="A35" s="4" t="s">
         <v>71</v>
       </c>
@@ -1180,7 +1208,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="19">
       <c r="A36" s="4" t="s">
         <v>35</v>
       </c>
@@ -1188,7 +1216,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="19">
       <c r="A37" s="4" t="s">
         <v>36</v>
       </c>
@@ -1196,7 +1224,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="19">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
@@ -1204,7 +1232,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="19">
       <c r="A39" s="4" t="s">
         <v>41</v>
       </c>
@@ -1212,7 +1240,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="19">
       <c r="A40" s="4" t="s">
         <v>43</v>
       </c>
@@ -1220,7 +1248,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="19">
       <c r="A41" s="4" t="s">
         <v>45</v>
       </c>
@@ -1228,7 +1256,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="19">
       <c r="A42" s="4" t="s">
         <v>47</v>
       </c>
@@ -1236,7 +1264,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="19">
       <c r="A43" s="4" t="s">
         <v>49</v>
       </c>
@@ -1244,7 +1272,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="19">
       <c r="A44" s="4" t="s">
         <v>51</v>
       </c>
@@ -1252,7 +1280,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="19">
       <c r="A45" s="4" t="s">
         <v>55</v>
       </c>
@@ -1260,7 +1288,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="19">
       <c r="A46" s="4" t="s">
         <v>68</v>
       </c>
@@ -1268,7 +1296,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="19">
       <c r="A48" s="2" t="s">
         <v>57</v>
       </c>
@@ -1281,7 +1309,7 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="19">
       <c r="A49" s="4" t="s">
         <v>58</v>
       </c>
@@ -1294,7 +1322,7 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="19">
       <c r="A50" s="3"/>
       <c r="B50" s="4" t="s">
         <v>59</v>
@@ -1307,7 +1335,7 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="19">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
         <v>60</v>
@@ -1320,7 +1348,7 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="19">
       <c r="A52" s="3"/>
       <c r="B52" s="4" t="s">
         <v>61</v>
@@ -1333,7 +1361,7 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="19">
       <c r="A53" s="4" t="s">
         <v>62</v>
       </c>
@@ -1346,7 +1374,7 @@
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="19">
       <c r="A54" s="4" t="s">
         <v>63</v>
       </c>
@@ -1366,6 +1394,11 @@
     <mergeCell ref="B7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1374,17 +1407,17 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="4" max="4" width="69.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -1404,7 +1437,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -1424,7 +1457,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -1444,7 +1477,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -1464,7 +1497,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -1484,7 +1517,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -1504,7 +1537,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -1524,7 +1557,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -1546,18 +1579,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W30"/>
+  <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -1573,7 +1612,7 @@
     <col min="22" max="22" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="19">
       <c r="A1" s="4" t="s">
         <v>74</v>
       </c>
@@ -1644,219 +1683,239 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" t="s">
         <v>75</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B16" t="s">
         <v>76</v>
       </c>
-      <c r="C2">
+      <c r="C16">
         <v>2013</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D16" t="s">
         <v>77</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E16" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G16" t="s">
         <v>80</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H16" t="s">
         <v>81</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I16" t="s">
         <v>82</v>
       </c>
-      <c r="J2">
+      <c r="J16">
         <v>-35</v>
       </c>
-      <c r="K2">
+      <c r="K16">
         <v>4</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L16" t="s">
         <v>112</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M16" t="s">
         <v>85</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N16" t="s">
         <v>86</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O16" t="s">
         <v>87</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P16" t="s">
         <v>85</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q16" t="s">
         <v>113</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R16" t="s">
         <v>87</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S16" t="s">
         <v>88</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T16" t="s">
         <v>85</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U16" t="s">
         <v>85</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V16" t="s">
         <v>85</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:W1">
+    <sortState ref="A2:W30">
+      <sortCondition ref="A1:A30"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1866,8 +1925,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated lit review and timeline script
</commit_message>
<xml_diff>
--- a/References /LitReview.xlsx
+++ b/References /LitReview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="12420" yWindow="0" windowWidth="16300" windowHeight="14100" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="162">
   <si>
     <t>Metadata by Cat:</t>
   </si>
@@ -448,6 +448,72 @@
   </si>
   <si>
     <t>fu12</t>
+  </si>
+  <si>
+    <t>xin16</t>
+  </si>
+  <si>
+    <t>Xin, Q.</t>
+  </si>
+  <si>
+    <t>Agricultural and Forest Meterology</t>
+  </si>
+  <si>
+    <t>A risk-benefit model to simulate vegetation spring onset in response to multi-decadal climate varitability: theoretical basis and applications from the Northern Hemisphere</t>
+  </si>
+  <si>
+    <t>139-163</t>
+  </si>
+  <si>
+    <t>10.1016/j.agrformet.2016.06.017</t>
+  </si>
+  <si>
+    <t>modelling spring onset</t>
+  </si>
+  <si>
+    <t>deciduous broadleaf forests, grasslands, evergreen needleleaf forests</t>
+  </si>
+  <si>
+    <t>excellent climate paper that integrates spring onset and budburst</t>
+  </si>
+  <si>
+    <t>augspurger09</t>
+  </si>
+  <si>
+    <t>Gu, L.</t>
+  </si>
+  <si>
+    <t>BioScience</t>
+  </si>
+  <si>
+    <t>The 2007 eastern US spring freeze: increased cold damage in a warming world?</t>
+  </si>
+  <si>
+    <t>253-262</t>
+  </si>
+  <si>
+    <t>10.1641/B580311</t>
+  </si>
+  <si>
+    <t>introduces concept of false spring to scientific community</t>
+  </si>
+  <si>
+    <t>Functional Ecology</t>
+  </si>
+  <si>
+    <t>Convergence of leaf-out towards minimum risk of freezing damage in temperate trees</t>
+  </si>
+  <si>
+    <t>1-11</t>
+  </si>
+  <si>
+    <t>10.1111/1365-2435.12623</t>
+  </si>
+  <si>
+    <t>historic data, observational, and experimental</t>
+  </si>
+  <si>
+    <t>Sorbus aucuparia, Prunus avium, Tilia platyphyllos, Acer psuedoplatanus, Fagus sylvatica</t>
   </si>
 </sst>
 </file>
@@ -531,8 +597,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -551,11 +621,15 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -823,7 +897,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -842,7 +916,7 @@
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -890,7 +964,7 @@
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="9" spans="1:9" ht="19">
+    <row r="9" spans="1:9" ht="18">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -902,7 +976,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="19">
+    <row r="10" spans="1:9" ht="18">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -916,7 +990,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="19">
+    <row r="11" spans="1:9" ht="18">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -930,7 +1004,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="19">
+    <row r="12" spans="1:9" ht="18">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -944,7 +1018,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="17">
+    <row r="13" spans="1:9" ht="16">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -954,7 +1028,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="19">
+    <row r="14" spans="1:9" ht="18">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -966,7 +1040,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="19">
+    <row r="15" spans="1:9" ht="18">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -980,7 +1054,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="19">
+    <row r="16" spans="1:9" ht="18">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -994,7 +1068,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="19">
+    <row r="17" spans="1:8" ht="18">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -1008,7 +1082,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="19">
+    <row r="18" spans="1:8" ht="18">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -1022,7 +1096,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="19">
+    <row r="19" spans="1:8" ht="18">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
@@ -1036,7 +1110,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="19">
+    <row r="20" spans="1:8" ht="18">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1050,7 +1124,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="17">
+    <row r="21" spans="1:8" ht="16">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1060,7 +1134,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="19">
+    <row r="22" spans="1:8" ht="18">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1072,7 +1146,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" ht="19">
+    <row r="23" spans="1:8" ht="18">
       <c r="A23" s="4" t="s">
         <v>74</v>
       </c>
@@ -1086,7 +1160,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="19">
+    <row r="24" spans="1:8" ht="18">
       <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
@@ -1100,7 +1174,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="19">
+    <row r="25" spans="1:8" ht="18">
       <c r="A25" s="4" t="s">
         <v>28</v>
       </c>
@@ -1112,7 +1186,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="19">
+    <row r="26" spans="1:8" ht="18">
       <c r="A26" s="4" t="s">
         <v>29</v>
       </c>
@@ -1124,7 +1198,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="19">
+    <row r="27" spans="1:8" ht="18">
       <c r="A27" s="4" t="s">
         <v>30</v>
       </c>
@@ -1136,7 +1210,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="19">
+    <row r="28" spans="1:8" ht="18">
       <c r="A28" s="4" t="s">
         <v>31</v>
       </c>
@@ -1148,7 +1222,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="19">
+    <row r="29" spans="1:8" ht="18">
       <c r="A29" s="4" t="s">
         <v>32</v>
       </c>
@@ -1160,7 +1234,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="19">
+    <row r="30" spans="1:8" ht="18">
       <c r="A30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1168,7 +1242,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="19">
+    <row r="31" spans="1:8" ht="18">
       <c r="A31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1176,7 +1250,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="19">
+    <row r="32" spans="1:8" ht="18">
       <c r="A32" s="4" t="s">
         <v>64</v>
       </c>
@@ -1184,7 +1258,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="19">
+    <row r="33" spans="1:9" ht="18">
       <c r="A33" s="4" t="s">
         <v>66</v>
       </c>
@@ -1192,7 +1266,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="19">
+    <row r="34" spans="1:9" ht="18">
       <c r="A34" s="4" t="s">
         <v>69</v>
       </c>
@@ -1200,7 +1274,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="19">
+    <row r="35" spans="1:9" ht="18">
       <c r="A35" s="4" t="s">
         <v>71</v>
       </c>
@@ -1208,7 +1282,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="19">
+    <row r="36" spans="1:9" ht="18">
       <c r="A36" s="4" t="s">
         <v>35</v>
       </c>
@@ -1216,7 +1290,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="19">
+    <row r="37" spans="1:9" ht="18">
       <c r="A37" s="4" t="s">
         <v>36</v>
       </c>
@@ -1224,7 +1298,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="19">
+    <row r="38" spans="1:9" ht="18">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
@@ -1232,7 +1306,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="19">
+    <row r="39" spans="1:9" ht="18">
       <c r="A39" s="4" t="s">
         <v>41</v>
       </c>
@@ -1240,7 +1314,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="19">
+    <row r="40" spans="1:9" ht="18">
       <c r="A40" s="4" t="s">
         <v>43</v>
       </c>
@@ -1248,7 +1322,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="19">
+    <row r="41" spans="1:9" ht="18">
       <c r="A41" s="4" t="s">
         <v>45</v>
       </c>
@@ -1256,7 +1330,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="19">
+    <row r="42" spans="1:9" ht="18">
       <c r="A42" s="4" t="s">
         <v>47</v>
       </c>
@@ -1264,7 +1338,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="19">
+    <row r="43" spans="1:9" ht="18">
       <c r="A43" s="4" t="s">
         <v>49</v>
       </c>
@@ -1272,7 +1346,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="19">
+    <row r="44" spans="1:9" ht="18">
       <c r="A44" s="4" t="s">
         <v>51</v>
       </c>
@@ -1280,7 +1354,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="19">
+    <row r="45" spans="1:9" ht="18">
       <c r="A45" s="4" t="s">
         <v>55</v>
       </c>
@@ -1288,7 +1362,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="19">
+    <row r="46" spans="1:9" ht="18">
       <c r="A46" s="4" t="s">
         <v>68</v>
       </c>
@@ -1296,7 +1370,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="19">
+    <row r="48" spans="1:9" ht="18">
       <c r="A48" s="2" t="s">
         <v>57</v>
       </c>
@@ -1309,7 +1383,7 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:9" ht="19">
+    <row r="49" spans="1:9" ht="18">
       <c r="A49" s="4" t="s">
         <v>58</v>
       </c>
@@ -1322,7 +1396,7 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" ht="19">
+    <row r="50" spans="1:9" ht="18">
       <c r="A50" s="3"/>
       <c r="B50" s="4" t="s">
         <v>59</v>
@@ -1335,7 +1409,7 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:9" ht="19">
+    <row r="51" spans="1:9" ht="18">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
         <v>60</v>
@@ -1348,7 +1422,7 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:9" ht="19">
+    <row r="52" spans="1:9" ht="18">
       <c r="A52" s="3"/>
       <c r="B52" s="4" t="s">
         <v>61</v>
@@ -1361,7 +1435,7 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="1:9" ht="19">
+    <row r="53" spans="1:9" ht="18">
       <c r="A53" s="4" t="s">
         <v>62</v>
       </c>
@@ -1374,7 +1448,7 @@
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="1:9" ht="19">
+    <row r="54" spans="1:9" ht="18">
       <c r="A54" s="4" t="s">
         <v>63</v>
       </c>
@@ -1417,7 +1491,7 @@
     <col min="4" max="4" width="69.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -1590,10 +1664,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W32"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1612,7 +1689,7 @@
     <col min="22" max="22" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="19">
+    <row r="1" spans="1:23" ht="18">
       <c r="A1" s="4" t="s">
         <v>74</v>
       </c>
@@ -1690,218 +1767,300 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10">
+        <v>2008</v>
+      </c>
+      <c r="D10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" t="s">
+        <v>152</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G10" t="s">
+        <v>154</v>
+      </c>
+      <c r="W10" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
+      <c r="A17" t="s">
         <v>75</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>76</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>2013</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>77</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>80</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H17" t="s">
         <v>81</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I17" t="s">
         <v>82</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <v>-35</v>
       </c>
-      <c r="K16">
+      <c r="K17">
         <v>4</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L17" t="s">
         <v>112</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M17" t="s">
         <v>85</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N17" t="s">
         <v>86</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O17" t="s">
         <v>87</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P17" t="s">
         <v>85</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q17" t="s">
         <v>113</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R17" t="s">
         <v>87</v>
       </c>
-      <c r="S16" t="s">
+      <c r="S17" t="s">
         <v>88</v>
       </c>
-      <c r="T16" t="s">
+      <c r="T17" t="s">
         <v>85</v>
       </c>
-      <c r="U16" t="s">
+      <c r="U17" t="s">
         <v>85</v>
       </c>
-      <c r="V16" t="s">
+      <c r="V17" t="s">
         <v>85</v>
       </c>
-      <c r="W16" t="s">
+      <c r="W17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+    <row r="18" spans="1:23">
+      <c r="A18" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18">
+        <v>2016</v>
+      </c>
+      <c r="D18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E18" t="s">
+        <v>157</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="G18" t="s">
+        <v>159</v>
+      </c>
+      <c r="H18" t="s">
+        <v>160</v>
+      </c>
+      <c r="I18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="A19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+    <row r="20" spans="1:23">
+      <c r="A20" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+    <row r="21" spans="1:23">
+      <c r="A21" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
+    <row r="22" spans="1:23">
+      <c r="A22" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
+    <row r="23" spans="1:23">
+      <c r="A23" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
+    <row r="24" spans="1:23">
+      <c r="A24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
+    <row r="25" spans="1:23">
+      <c r="A25" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
+    <row r="26" spans="1:23">
+      <c r="A26" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
+    <row r="27" spans="1:23">
+      <c r="A27" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
+    <row r="28" spans="1:23">
+      <c r="A28" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
+    <row r="29" spans="1:23">
+      <c r="A29" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
+    <row r="30" spans="1:23">
+      <c r="A30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:23">
       <c r="A31" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:23">
       <c r="A32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
+      <c r="A33" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="A34" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C34">
+        <v>2016</v>
+      </c>
+      <c r="D34" t="s">
+        <v>142</v>
+      </c>
+      <c r="E34" t="s">
+        <v>143</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="G34" t="s">
+        <v>145</v>
+      </c>
+      <c r="H34" t="s">
+        <v>146</v>
+      </c>
+      <c r="I34" t="s">
+        <v>147</v>
+      </c>
+      <c r="W34" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1911,6 +2070,7 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>